<commit_message>
feat(data): merge Bus 61 routes and update app config
</commit_message>
<xml_diff>
--- a/data/bus_routes.xlsx
+++ b/data/bus_routes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -712,6 +712,804 @@
         <v>85.828</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>61</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>KIIT Transport Department</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>20.3555</v>
+      </c>
+      <c r="E14" t="n">
+        <v>85.81950000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>61</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>KIIT Campus 6</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>20.356</v>
+      </c>
+      <c r="E15" t="n">
+        <v>85.82000000000001</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>61</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>KIIT Campus 3</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>20.3565</v>
+      </c>
+      <c r="E16" t="n">
+        <v>85.8205</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>61</v>
+      </c>
+      <c r="B17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>KIIMS</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>20.357</v>
+      </c>
+      <c r="E17" t="n">
+        <v>85.821</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>61</v>
+      </c>
+      <c r="B18" t="n">
+        <v>5</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>KIIT International School</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>20.3575</v>
+      </c>
+      <c r="E18" t="n">
+        <v>85.8215</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>61</v>
+      </c>
+      <c r="B19" t="n">
+        <v>6</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Silicon University</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>20.358</v>
+      </c>
+      <c r="E19" t="n">
+        <v>85.822</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>61</v>
+      </c>
+      <c r="B20" t="n">
+        <v>7</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>DLF Cyber City</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>20.3585</v>
+      </c>
+      <c r="E20" t="n">
+        <v>85.82250000000001</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>61</v>
+      </c>
+      <c r="B21" t="n">
+        <v>8</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Infocity Square</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>20.359</v>
+      </c>
+      <c r="E21" t="n">
+        <v>85.82300000000001</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>61</v>
+      </c>
+      <c r="B22" t="n">
+        <v>9</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Lord Jagannath Temple Sailashree Vihar</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>20.3595</v>
+      </c>
+      <c r="E22" t="n">
+        <v>85.8235</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>61</v>
+      </c>
+      <c r="B23" t="n">
+        <v>10</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Powergrid ER2 Odisha Projects</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>20.36</v>
+      </c>
+      <c r="E23" t="n">
+        <v>85.824</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>61</v>
+      </c>
+      <c r="B24" t="n">
+        <v>11</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Utkal Hospital</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>20.3605</v>
+      </c>
+      <c r="E24" t="n">
+        <v>85.8245</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>61</v>
+      </c>
+      <c r="B25" t="n">
+        <v>12</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Rail Vihar Road</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>20.361</v>
+      </c>
+      <c r="E25" t="n">
+        <v>85.825</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>61</v>
+      </c>
+      <c r="B26" t="n">
+        <v>13</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Kalinga Hospital Chowk</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>20.3615</v>
+      </c>
+      <c r="E26" t="n">
+        <v>85.82550000000001</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>61</v>
+      </c>
+      <c r="B27" t="n">
+        <v>14</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Allen Career Institute</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>20.362</v>
+      </c>
+      <c r="E27" t="n">
+        <v>85.82600000000001</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>61</v>
+      </c>
+      <c r="B28" t="n">
+        <v>15</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Janta Maidan</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>20.3625</v>
+      </c>
+      <c r="E28" t="n">
+        <v>85.8265</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>61</v>
+      </c>
+      <c r="B29" t="n">
+        <v>16</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Pal Heights Mall</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>20.363</v>
+      </c>
+      <c r="E29" t="n">
+        <v>85.827</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>61</v>
+      </c>
+      <c r="B30" t="n">
+        <v>17</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Kalinga Stadium</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>20.3635</v>
+      </c>
+      <c r="E30" t="n">
+        <v>85.8275</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>61</v>
+      </c>
+      <c r="B31" t="n">
+        <v>18</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Raj Bhavan</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>20.364</v>
+      </c>
+      <c r="E31" t="n">
+        <v>85.828</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>61</v>
+      </c>
+      <c r="B32" t="n">
+        <v>19</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Bana Durga Temple Road</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>20.3645</v>
+      </c>
+      <c r="E32" t="n">
+        <v>85.82850000000001</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>61</v>
+      </c>
+      <c r="B33" t="n">
+        <v>20</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Ekamra Road</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>20.365</v>
+      </c>
+      <c r="E33" t="n">
+        <v>85.82900000000001</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>61</v>
+      </c>
+      <c r="B34" t="n">
+        <v>21</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Forest Park</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>20.3655</v>
+      </c>
+      <c r="E34" t="n">
+        <v>85.8295</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>61</v>
+      </c>
+      <c r="B35" t="n">
+        <v>22</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Janpath Road</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>20.366</v>
+      </c>
+      <c r="E35" t="n">
+        <v>85.83</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>61</v>
+      </c>
+      <c r="B36" t="n">
+        <v>23</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Rajmahal Flyover</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>20.3665</v>
+      </c>
+      <c r="E36" t="n">
+        <v>85.8305</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>61</v>
+      </c>
+      <c r="B37" t="n">
+        <v>24</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Bhubaneswar Railway Station (Master Canteen)</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>20.367</v>
+      </c>
+      <c r="E37" t="n">
+        <v>85.831</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>61</v>
+      </c>
+      <c r="B38" t="n">
+        <v>25</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Sriya Square</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>20.3675</v>
+      </c>
+      <c r="E38" t="n">
+        <v>85.83150000000001</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>61</v>
+      </c>
+      <c r="B39" t="n">
+        <v>26</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Shree Ram Temple</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>20.368</v>
+      </c>
+      <c r="E39" t="n">
+        <v>85.83200000000001</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>61</v>
+      </c>
+      <c r="B40" t="n">
+        <v>27</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Satya Nagar</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>20.3685</v>
+      </c>
+      <c r="E40" t="n">
+        <v>85.8325</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>61</v>
+      </c>
+      <c r="B41" t="n">
+        <v>28</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Rupali Square</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>20.369</v>
+      </c>
+      <c r="E41" t="n">
+        <v>85.833</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>61</v>
+      </c>
+      <c r="B42" t="n">
+        <v>29</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Vani Vihar</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>20.3695</v>
+      </c>
+      <c r="E42" t="n">
+        <v>85.8335</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>61</v>
+      </c>
+      <c r="B43" t="n">
+        <v>30</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Pathani Samanta Planetarium</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>20.37</v>
+      </c>
+      <c r="E43" t="n">
+        <v>85.834</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>61</v>
+      </c>
+      <c r="B44" t="n">
+        <v>31</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Sainik School Road</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>20.3705</v>
+      </c>
+      <c r="E44" t="n">
+        <v>85.83450000000001</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>61</v>
+      </c>
+      <c r="B45" t="n">
+        <v>32</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Zaika Palace North Indian</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>20.371</v>
+      </c>
+      <c r="E45" t="n">
+        <v>85.83500000000001</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>61</v>
+      </c>
+      <c r="B46" t="n">
+        <v>33</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Barbeque Nation Sachivalaya Marg</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>20.3715</v>
+      </c>
+      <c r="E46" t="n">
+        <v>85.8355</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>61</v>
+      </c>
+      <c r="B47" t="n">
+        <v>34</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Care Hospital Square</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>20.372</v>
+      </c>
+      <c r="E47" t="n">
+        <v>85.836</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>61</v>
+      </c>
+      <c r="B48" t="n">
+        <v>35</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Damana Square</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>20.3725</v>
+      </c>
+      <c r="E48" t="n">
+        <v>85.8365</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>61</v>
+      </c>
+      <c r="B49" t="n">
+        <v>36</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Patia Chowk</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>20.373</v>
+      </c>
+      <c r="E49" t="n">
+        <v>85.837</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>61</v>
+      </c>
+      <c r="B50" t="n">
+        <v>37</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>KIIT Campus 1 (Koel)</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>20.3735</v>
+      </c>
+      <c r="E50" t="n">
+        <v>85.83750000000001</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>61</v>
+      </c>
+      <c r="B51" t="n">
+        <v>38</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>KIIT Square</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>20.374</v>
+      </c>
+      <c r="E51" t="n">
+        <v>85.83800000000001</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>61</v>
+      </c>
+      <c r="B52" t="n">
+        <v>39</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>KIIT Campus 6</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>20.3745</v>
+      </c>
+      <c r="E52" t="n">
+        <v>85.8385</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>61</v>
+      </c>
+      <c r="B53" t="n">
+        <v>40</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>KIIT Campus 3</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>20.375</v>
+      </c>
+      <c r="E53" t="n">
+        <v>85.839</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>61</v>
+      </c>
+      <c r="B54" t="n">
+        <v>41</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>KIIT Campus 14</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>20.3755</v>
+      </c>
+      <c r="E54" t="n">
+        <v>85.8395</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>61</v>
+      </c>
+      <c r="B55" t="n">
+        <v>42</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>KIIT Campus 25</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>20.376</v>
+      </c>
+      <c r="E55" t="n">
+        <v>85.84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(ui): refactor header layout and cleanup dead code
</commit_message>
<xml_diff>
--- a/data/bus_routes.xlsx
+++ b/data/bus_routes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>61</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -471,20 +471,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Master Canteen</t>
+          <t>KIIT Transport Department</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>20.2667</v>
+        <v>20.3555</v>
       </c>
       <c r="E2" t="n">
-        <v>85.843</v>
+        <v>85.81950000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>61</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -492,20 +492,20 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Rajmahal</t>
+          <t>KIIT Campus 6</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>20.27</v>
+        <v>20.356</v>
       </c>
       <c r="E3" t="n">
-        <v>85.83499999999999</v>
+        <v>85.82000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>61</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -513,77 +513,77 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Airport</t>
+          <t>KIIT Campus 3</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>20.255</v>
+        <v>20.3565</v>
       </c>
       <c r="E4" t="n">
-        <v>85.815</v>
+        <v>85.8205</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>EV-1</t>
+          <t>61</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Admin Block</t>
+          <t>KIIMS</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>20.2961</v>
+        <v>20.357</v>
       </c>
       <c r="E5" t="n">
-        <v>85.8245</v>
+        <v>85.821</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EV-1</t>
+          <t>61</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Library</t>
+          <t>KIIT International School</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>20.298</v>
+        <v>20.3575</v>
       </c>
       <c r="E6" t="n">
-        <v>85.82599999999999</v>
+        <v>85.8215</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EV-1</t>
+          <t>61</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hostel 1</t>
+          <t>Silicon University</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>20.3</v>
+        <v>20.358</v>
       </c>
       <c r="E7" t="n">
-        <v>85.828</v>
+        <v>85.822</v>
       </c>
     </row>
     <row r="8">
@@ -593,18 +593,18 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>KIIT Transport Department</t>
+          <t>DLF Cyber City</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>20.3555</v>
+        <v>20.3585</v>
       </c>
       <c r="E8" t="n">
-        <v>85.81950000000001</v>
+        <v>85.82250000000001</v>
       </c>
     </row>
     <row r="9">
@@ -614,18 +614,18 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>KIIT Campus 6</t>
+          <t>Infocity Square</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>20.356</v>
+        <v>20.359</v>
       </c>
       <c r="E9" t="n">
-        <v>85.82000000000001</v>
+        <v>85.82300000000001</v>
       </c>
     </row>
     <row r="10">
@@ -635,18 +635,18 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>KIIT Campus 3</t>
+          <t>Lord Jagannath Temple Sailashree Vihar</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>20.3565</v>
+        <v>20.3595</v>
       </c>
       <c r="E10" t="n">
-        <v>85.8205</v>
+        <v>85.8235</v>
       </c>
     </row>
     <row r="11">
@@ -656,18 +656,18 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>KIIMS</t>
+          <t>Powergrid ER2 Odisha Projects</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>20.357</v>
+        <v>20.36</v>
       </c>
       <c r="E11" t="n">
-        <v>85.821</v>
+        <v>85.824</v>
       </c>
     </row>
     <row r="12">
@@ -677,18 +677,18 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>KIIT International School</t>
+          <t>Utkal Hospital</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>20.3575</v>
+        <v>20.3605</v>
       </c>
       <c r="E12" t="n">
-        <v>85.8215</v>
+        <v>85.8245</v>
       </c>
     </row>
     <row r="13">
@@ -698,18 +698,18 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Silicon University</t>
+          <t>Rail Vihar Road</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>20.358</v>
+        <v>20.361</v>
       </c>
       <c r="E13" t="n">
-        <v>85.822</v>
+        <v>85.825</v>
       </c>
     </row>
     <row r="14">
@@ -719,18 +719,18 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>DLF Cyber City</t>
+          <t>Kalinga Hospital Chowk</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>20.3585</v>
+        <v>20.3615</v>
       </c>
       <c r="E14" t="n">
-        <v>85.82250000000001</v>
+        <v>85.82550000000001</v>
       </c>
     </row>
     <row r="15">
@@ -740,18 +740,18 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Infocity Square</t>
+          <t>Allen Career Institute</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>20.359</v>
+        <v>20.362</v>
       </c>
       <c r="E15" t="n">
-        <v>85.82300000000001</v>
+        <v>85.82600000000001</v>
       </c>
     </row>
     <row r="16">
@@ -761,18 +761,18 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Lord Jagannath Temple Sailashree Vihar</t>
+          <t>Janta Maidan</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>20.3595</v>
+        <v>20.3625</v>
       </c>
       <c r="E16" t="n">
-        <v>85.8235</v>
+        <v>85.8265</v>
       </c>
     </row>
     <row r="17">
@@ -782,18 +782,18 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Powergrid ER2 Odisha Projects</t>
+          <t>Pal Heights Mall</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>20.36</v>
+        <v>20.363</v>
       </c>
       <c r="E17" t="n">
-        <v>85.824</v>
+        <v>85.827</v>
       </c>
     </row>
     <row r="18">
@@ -803,18 +803,18 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Utkal Hospital</t>
+          <t>Kalinga Stadium</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>20.3605</v>
+        <v>20.3635</v>
       </c>
       <c r="E18" t="n">
-        <v>85.8245</v>
+        <v>85.8275</v>
       </c>
     </row>
     <row r="19">
@@ -824,18 +824,18 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Rail Vihar Road</t>
+          <t>Raj Bhavan</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>20.361</v>
+        <v>20.364</v>
       </c>
       <c r="E19" t="n">
-        <v>85.825</v>
+        <v>85.828</v>
       </c>
     </row>
     <row r="20">
@@ -845,18 +845,18 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Kalinga Hospital Chowk</t>
+          <t>Bana Durga Temple Road</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>20.3615</v>
+        <v>20.3645</v>
       </c>
       <c r="E20" t="n">
-        <v>85.82550000000001</v>
+        <v>85.82850000000001</v>
       </c>
     </row>
     <row r="21">
@@ -866,18 +866,18 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Allen Career Institute</t>
+          <t>Ekamra Road</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>20.362</v>
+        <v>20.365</v>
       </c>
       <c r="E21" t="n">
-        <v>85.82600000000001</v>
+        <v>85.82900000000001</v>
       </c>
     </row>
     <row r="22">
@@ -887,18 +887,18 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Janta Maidan</t>
+          <t>Forest Park</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>20.3625</v>
+        <v>20.3655</v>
       </c>
       <c r="E22" t="n">
-        <v>85.8265</v>
+        <v>85.8295</v>
       </c>
     </row>
     <row r="23">
@@ -908,18 +908,18 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Pal Heights Mall</t>
+          <t>Janpath Road</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>20.363</v>
+        <v>20.366</v>
       </c>
       <c r="E23" t="n">
-        <v>85.827</v>
+        <v>85.83</v>
       </c>
     </row>
     <row r="24">
@@ -929,18 +929,18 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Kalinga Stadium</t>
+          <t>Rajmahal Flyover</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>20.3635</v>
+        <v>20.3665</v>
       </c>
       <c r="E24" t="n">
-        <v>85.8275</v>
+        <v>85.8305</v>
       </c>
     </row>
     <row r="25">
@@ -950,18 +950,18 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Raj Bhavan</t>
+          <t>Bhubaneswar Railway Station (Master Canteen)</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>20.364</v>
+        <v>20.367</v>
       </c>
       <c r="E25" t="n">
-        <v>85.828</v>
+        <v>85.831</v>
       </c>
     </row>
     <row r="26">
@@ -971,18 +971,18 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bana Durga Temple Road</t>
+          <t>Sriya Square</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>20.3645</v>
+        <v>20.3675</v>
       </c>
       <c r="E26" t="n">
-        <v>85.82850000000001</v>
+        <v>85.83150000000001</v>
       </c>
     </row>
     <row r="27">
@@ -992,18 +992,18 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Ekamra Road</t>
+          <t>Shree Ram Temple</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>20.365</v>
+        <v>20.368</v>
       </c>
       <c r="E27" t="n">
-        <v>85.82900000000001</v>
+        <v>85.83200000000001</v>
       </c>
     </row>
     <row r="28">
@@ -1013,18 +1013,18 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Forest Park</t>
+          <t>Satya Nagar</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>20.3655</v>
+        <v>20.3685</v>
       </c>
       <c r="E28" t="n">
-        <v>85.8295</v>
+        <v>85.8325</v>
       </c>
     </row>
     <row r="29">
@@ -1034,18 +1034,18 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Janpath Road</t>
+          <t>Rupali Square</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>20.366</v>
+        <v>20.369</v>
       </c>
       <c r="E29" t="n">
-        <v>85.83</v>
+        <v>85.833</v>
       </c>
     </row>
     <row r="30">
@@ -1055,18 +1055,18 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Rajmahal Flyover</t>
+          <t>Vani Vihar</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>20.3665</v>
+        <v>20.3695</v>
       </c>
       <c r="E30" t="n">
-        <v>85.8305</v>
+        <v>85.8335</v>
       </c>
     </row>
     <row r="31">
@@ -1076,18 +1076,18 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Bhubaneswar Railway Station (Master Canteen)</t>
+          <t>Pathani Samanta Planetarium</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>20.367</v>
+        <v>20.37</v>
       </c>
       <c r="E31" t="n">
-        <v>85.831</v>
+        <v>85.834</v>
       </c>
     </row>
     <row r="32">
@@ -1097,18 +1097,18 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Sriya Square</t>
+          <t>Sainik School Road</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>20.3675</v>
+        <v>20.3705</v>
       </c>
       <c r="E32" t="n">
-        <v>85.83150000000001</v>
+        <v>85.83450000000001</v>
       </c>
     </row>
     <row r="33">
@@ -1118,18 +1118,18 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Shree Ram Temple</t>
+          <t>Zaika Palace North Indian</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>20.368</v>
+        <v>20.371</v>
       </c>
       <c r="E33" t="n">
-        <v>85.83200000000001</v>
+        <v>85.83500000000001</v>
       </c>
     </row>
     <row r="34">
@@ -1139,18 +1139,18 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Satya Nagar</t>
+          <t>Barbeque Nation Sachivalaya Marg</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>20.3685</v>
+        <v>20.3715</v>
       </c>
       <c r="E34" t="n">
-        <v>85.8325</v>
+        <v>85.8355</v>
       </c>
     </row>
     <row r="35">
@@ -1160,18 +1160,18 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Rupali Square</t>
+          <t>Care Hospital Square</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>20.369</v>
+        <v>20.372</v>
       </c>
       <c r="E35" t="n">
-        <v>85.833</v>
+        <v>85.836</v>
       </c>
     </row>
     <row r="36">
@@ -1181,18 +1181,18 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Vani Vihar</t>
+          <t>Damana Square</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>20.3695</v>
+        <v>20.3725</v>
       </c>
       <c r="E36" t="n">
-        <v>85.8335</v>
+        <v>85.8365</v>
       </c>
     </row>
     <row r="37">
@@ -1202,18 +1202,18 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Pathani Samanta Planetarium</t>
+          <t>Patia Chowk</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>20.37</v>
+        <v>20.373</v>
       </c>
       <c r="E37" t="n">
-        <v>85.834</v>
+        <v>85.837</v>
       </c>
     </row>
     <row r="38">
@@ -1223,18 +1223,18 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Sainik School Road</t>
+          <t>KIIT Campus 1 (Koel)</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>20.3705</v>
+        <v>20.3735</v>
       </c>
       <c r="E38" t="n">
-        <v>85.83450000000001</v>
+        <v>85.83750000000001</v>
       </c>
     </row>
     <row r="39">
@@ -1244,18 +1244,18 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Zaika Palace North Indian</t>
+          <t>KIIT Square</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>20.371</v>
+        <v>20.374</v>
       </c>
       <c r="E39" t="n">
-        <v>85.83500000000001</v>
+        <v>85.83800000000001</v>
       </c>
     </row>
     <row r="40">
@@ -1265,18 +1265,18 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Barbeque Nation Sachivalaya Marg</t>
+          <t>KIIT Campus 6</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>20.3715</v>
+        <v>20.3745</v>
       </c>
       <c r="E40" t="n">
-        <v>85.8355</v>
+        <v>85.8385</v>
       </c>
     </row>
     <row r="41">
@@ -1286,18 +1286,18 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Care Hospital Square</t>
+          <t>KIIT Campus 3</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>20.372</v>
+        <v>20.375</v>
       </c>
       <c r="E41" t="n">
-        <v>85.836</v>
+        <v>85.839</v>
       </c>
     </row>
     <row r="42">
@@ -1307,18 +1307,18 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Damana Square</t>
+          <t>KIIT Campus 14</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>20.3725</v>
+        <v>20.3755</v>
       </c>
       <c r="E42" t="n">
-        <v>85.8365</v>
+        <v>85.8395</v>
       </c>
     </row>
     <row r="43">
@@ -1328,143 +1328,17 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Patia Chowk</t>
+          <t>KIIT Campus 25</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>20.373</v>
+        <v>20.376</v>
       </c>
       <c r="E43" t="n">
-        <v>85.837</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>37</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>KIIT Campus 1 (Koel)</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>20.3735</v>
-      </c>
-      <c r="E44" t="n">
-        <v>85.83750000000001</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>38</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>KIIT Square</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>20.374</v>
-      </c>
-      <c r="E45" t="n">
-        <v>85.83800000000001</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>39</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>KIIT Campus 6</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>20.3745</v>
-      </c>
-      <c r="E46" t="n">
-        <v>85.8385</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>40</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>KIIT Campus 3</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>20.375</v>
-      </c>
-      <c r="E47" t="n">
-        <v>85.839</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>41</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>KIIT Campus 14</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>20.3755</v>
-      </c>
-      <c r="E48" t="n">
-        <v>85.8395</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>42</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>KIIT Campus 25</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>20.376</v>
-      </c>
-      <c r="E49" t="n">
         <v>85.84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(data): update all bus routes and coordinates
</commit_message>
<xml_diff>
--- a/data/bus_routes.xlsx
+++ b/data/bus_routes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -471,20 +471,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>KIIT Transport Department</t>
+          <t>KIIT Campus 25 (Computer Science)</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>20.3555</v>
+        <v>20.3585</v>
       </c>
       <c r="E2" t="n">
-        <v>85.81950000000001</v>
+        <v>85.813</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -492,20 +492,20 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>KIIT Campus 6</t>
+          <t>KIIT Square</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>20.356</v>
+        <v>20.351</v>
       </c>
       <c r="E3" t="n">
-        <v>85.82000000000001</v>
+        <v>85.8189</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -513,20 +513,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>KIIT Campus 3</t>
+          <t>Patia Square</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>20.3565</v>
+        <v>20.3444</v>
       </c>
       <c r="E4" t="n">
-        <v>85.8205</v>
+        <v>85.8164</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -534,20 +534,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>KIIMS</t>
+          <t>Damana Square</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>20.357</v>
+        <v>20.334</v>
       </c>
       <c r="E5" t="n">
-        <v>85.821</v>
+        <v>85.8175</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -555,20 +555,20 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>KIIT International School</t>
+          <t>Acharya Vihar (NH)</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>20.3575</v>
+        <v>20.294</v>
       </c>
       <c r="E6" t="n">
-        <v>85.8215</v>
+        <v>85.8395</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -576,20 +576,20 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Silicon University</t>
+          <t>Vani Vihar (NH)</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>20.358</v>
+        <v>20.2905</v>
       </c>
       <c r="E7" t="n">
-        <v>85.822</v>
+        <v>85.84699999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -597,20 +597,20 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>DLF Cyber City</t>
+          <t>Rasulgarh Square</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>20.3585</v>
+        <v>20.2885</v>
       </c>
       <c r="E8" t="n">
-        <v>85.82250000000001</v>
+        <v>85.86450000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -618,20 +618,20 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Infocity Square</t>
+          <t>Pahal</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>20.359</v>
+        <v>20.342</v>
       </c>
       <c r="E9" t="n">
-        <v>85.82300000000001</v>
+        <v>85.895</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -639,20 +639,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Lord Jagannath Temple Sailashree Vihar</t>
+          <t>Phulnakhara</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>20.3595</v>
+        <v>20.365</v>
       </c>
       <c r="E10" t="n">
-        <v>85.8235</v>
+        <v>85.91800000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -660,20 +660,20 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Powergrid ER2 Odisha Projects</t>
+          <t>Link Road (Cuttack)</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>20.36</v>
+        <v>20.443</v>
       </c>
       <c r="E11" t="n">
-        <v>85.824</v>
+        <v>85.88500000000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -681,665 +681,1820 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Utkal Hospital</t>
+          <t>Badambadi Bus Stand (Cuttack)</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>20.3605</v>
+        <v>20.452</v>
       </c>
       <c r="E12" t="n">
-        <v>85.8245</v>
+        <v>85.875</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Rail Vihar Road</t>
+          <t>KIIT Campus 25 (End)</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>20.361</v>
+        <v>20.3585</v>
       </c>
       <c r="E13" t="n">
-        <v>85.825</v>
+        <v>85.813</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Kalinga Hospital Chowk</t>
+          <t>KIIT Campus 25 (Computer Science)</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>20.3615</v>
+        <v>20.3585</v>
       </c>
       <c r="E14" t="n">
-        <v>85.82550000000001</v>
+        <v>85.813</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Allen Career Institute</t>
+          <t>KIIT Transport Office</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>20.362</v>
+        <v>20.3524</v>
       </c>
       <c r="E15" t="n">
-        <v>85.82600000000001</v>
+        <v>85.8182</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Janta Maidan</t>
+          <t>KIIT Square</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>20.3625</v>
+        <v>20.351</v>
       </c>
       <c r="E16" t="n">
-        <v>85.8265</v>
+        <v>85.8189</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Pal Heights Mall</t>
+          <t>KIIT Campus 6</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>20.363</v>
+        <v>20.352</v>
       </c>
       <c r="E17" t="n">
-        <v>85.827</v>
+        <v>85.818</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Kalinga Stadium</t>
+          <t>KIIT Campus 3</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>20.3635</v>
+        <v>20.3501</v>
       </c>
       <c r="E18" t="n">
-        <v>85.8275</v>
+        <v>85.81659999999999</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Raj Bhavan</t>
+          <t>KP 7 (Kings Palace 7)</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>20.364</v>
+        <v>20.354</v>
       </c>
       <c r="E19" t="n">
-        <v>85.828</v>
+        <v>85.816</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bana Durga Temple Road</t>
+          <t>KIIT Campus 3 (Return)</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>20.3645</v>
+        <v>20.3503</v>
       </c>
       <c r="E20" t="n">
-        <v>85.82850000000001</v>
+        <v>85.8168</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Ekamra Road</t>
+          <t>KIIT Campus 6 (Return)</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>20.365</v>
+        <v>20.3522</v>
       </c>
       <c r="E21" t="n">
-        <v>85.82900000000001</v>
+        <v>85.8182</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Forest Park</t>
+          <t>KIIT Square (Return)</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>20.3655</v>
+        <v>20.3512</v>
       </c>
       <c r="E22" t="n">
-        <v>85.8295</v>
+        <v>85.81910000000001</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Janpath Road</t>
+          <t>KIIT Transport Office (Return)</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>20.366</v>
+        <v>20.3526</v>
       </c>
       <c r="E23" t="n">
-        <v>85.83</v>
+        <v>85.8184</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Rajmahal Flyover</t>
+          <t>KIIT Campus 25 (Computer Science) End</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>20.3665</v>
+        <v>20.3585</v>
       </c>
       <c r="E24" t="n">
-        <v>85.8305</v>
+        <v>85.813</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Bhubaneswar Railway Station (Master Canteen)</t>
+          <t>KIIT Transport Department</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>20.367</v>
+        <v>20.3524</v>
       </c>
       <c r="E25" t="n">
-        <v>85.831</v>
+        <v>85.8182</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Sriya Square</t>
+          <t>KIIT Campus 6</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>20.3675</v>
+        <v>20.3508</v>
       </c>
       <c r="E26" t="n">
-        <v>85.83150000000001</v>
+        <v>85.8185</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Shree Ram Temple</t>
+          <t>KIIT Campus 3</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>20.368</v>
+        <v>20.3501</v>
       </c>
       <c r="E27" t="n">
-        <v>85.83200000000001</v>
+        <v>85.81659999999999</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Satya Nagar</t>
+          <t>KIMS</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>20.3685</v>
+        <v>20.3495</v>
       </c>
       <c r="E28" t="n">
-        <v>85.8325</v>
+        <v>85.81529999999999</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Rupali Square</t>
+          <t>KIIT International School</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>20.369</v>
+        <v>20.3425</v>
       </c>
       <c r="E29" t="n">
-        <v>85.833</v>
+        <v>85.81399999999999</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Vani Vihar</t>
+          <t>Silicon University</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>20.3695</v>
+        <v>20.3513</v>
       </c>
       <c r="E30" t="n">
-        <v>85.8335</v>
+        <v>85.80540000000001</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Pathani Samanta Planetarium</t>
+          <t>DLF Cyber City</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>20.37</v>
+        <v>20.3552</v>
       </c>
       <c r="E31" t="n">
-        <v>85.834</v>
+        <v>85.8105</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Sainik School Road</t>
+          <t>Infocity Square</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>20.3705</v>
+        <v>20.3568</v>
       </c>
       <c r="E32" t="n">
-        <v>85.83450000000001</v>
+        <v>85.8078</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Zaika Palace North Indian</t>
+          <t>Lord Jagannath Temple</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>20.371</v>
+        <v>20.3452</v>
       </c>
       <c r="E33" t="n">
-        <v>85.83500000000001</v>
+        <v>85.81950000000001</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Barbeque Nation Sachivalaya Marg</t>
+          <t>Powergrid</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>20.3715</v>
+        <v>20.3345</v>
       </c>
       <c r="E34" t="n">
-        <v>85.8355</v>
+        <v>85.8202</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Care Hospital Square</t>
+          <t>Utkal Hospital</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>20.372</v>
+        <v>20.3242</v>
       </c>
       <c r="E35" t="n">
-        <v>85.836</v>
+        <v>85.8188</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Damana Square</t>
+          <t>Rail Vihar Road</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>20.3725</v>
+        <v>20.3225</v>
       </c>
       <c r="E36" t="n">
-        <v>85.8365</v>
+        <v>85.8192</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Patia Chowk</t>
+          <t>Kalinga Hospital Chowk</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>20.373</v>
+        <v>20.3204</v>
       </c>
       <c r="E37" t="n">
-        <v>85.837</v>
+        <v>85.8197</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>KIIT Campus 1 (Koel)</t>
+          <t>Allen Career Institute</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>20.3735</v>
+        <v>20.3122</v>
       </c>
       <c r="E38" t="n">
-        <v>85.83750000000001</v>
+        <v>85.8248</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>KIIT Square</t>
+          <t>Janta Maidan</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>20.374</v>
+        <v>20.3065</v>
       </c>
       <c r="E39" t="n">
-        <v>85.83800000000001</v>
+        <v>85.8265</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>KIIT Campus 6</t>
+          <t>Pal Heights Mall</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>20.3745</v>
+        <v>20.2982</v>
       </c>
       <c r="E40" t="n">
-        <v>85.8385</v>
+        <v>85.8185</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>KIIT Campus 3</t>
+          <t>Kalinga Stadium</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>20.375</v>
+        <v>20.2905</v>
       </c>
       <c r="E41" t="n">
-        <v>85.839</v>
+        <v>85.8201</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>KIIT Campus 14</t>
+          <t>Raj Bhavan</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>20.3755</v>
+        <v>20.2785</v>
       </c>
       <c r="E42" t="n">
-        <v>85.8395</v>
+        <v>85.82250000000001</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>19</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Bana Durga Temple Road</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>20.2732</v>
+      </c>
+      <c r="E43" t="n">
+        <v>85.82550000000001</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>20</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Ekamra Niwas</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>20.2715</v>
+      </c>
+      <c r="E44" t="n">
+        <v>85.8288</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>21</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>AG Square</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>20.268</v>
+      </c>
+      <c r="E45" t="n">
+        <v>85.83199999999999</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>22</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Capital Hospital</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>20.2625</v>
+      </c>
+      <c r="E46" t="n">
+        <v>85.825</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>KIIT Transport Office</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>20.3524</v>
+      </c>
+      <c r="E47" t="n">
+        <v>85.8182</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>KIIT Square</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>20.3508</v>
+      </c>
+      <c r="E48" t="n">
+        <v>85.8185</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>3</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Patia Square</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>20.3444</v>
+      </c>
+      <c r="E49" t="n">
+        <v>85.8164</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>4</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Damana Square</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>20.334</v>
+      </c>
+      <c r="E50" t="n">
+        <v>85.8175</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>5</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Chandrasekharpur</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>20.3245</v>
+      </c>
+      <c r="E51" t="n">
+        <v>85.8185</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>6</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Niladri Vihar Square</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>20.316</v>
+      </c>
+      <c r="E52" t="n">
+        <v>85.819</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>7</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>VSS Nagar</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>20.301</v>
+      </c>
+      <c r="E53" t="n">
+        <v>85.845</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>8</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Rasulgarh Square</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>20.2885</v>
+      </c>
+      <c r="E54" t="n">
+        <v>85.86450000000001</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>9</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>VSS Nagar (Return)</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>20.3015</v>
+      </c>
+      <c r="E55" t="n">
+        <v>85.8455</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>10</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Niladri Vihar (Return)</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>20.3165</v>
+      </c>
+      <c r="E56" t="n">
+        <v>85.81950000000001</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>11</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Chandrasekharpur (Return)</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>20.325</v>
+      </c>
+      <c r="E57" t="n">
+        <v>85.819</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>12</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Damana Square (Return)</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>20.3345</v>
+      </c>
+      <c r="E58" t="n">
+        <v>85.818</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>13</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Patia Square (Return)</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>20.3448</v>
+      </c>
+      <c r="E59" t="n">
+        <v>85.8168</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>14</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>KIIT Square (Return)</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>20.351</v>
+      </c>
+      <c r="E60" t="n">
+        <v>85.819</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>15</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>KIIT Campus 25</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>20.3585</v>
+      </c>
+      <c r="E61" t="n">
+        <v>85.813</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>KIIT Transport Office</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>20.3524</v>
+      </c>
+      <c r="E62" t="n">
+        <v>85.8182</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>2</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>KIIT Square</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>20.3508</v>
+      </c>
+      <c r="E63" t="n">
+        <v>85.8185</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>3</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Patia Square</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>20.3444</v>
+      </c>
+      <c r="E64" t="n">
+        <v>85.8164</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>4</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Damana Square</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>20.334</v>
+      </c>
+      <c r="E65" t="n">
+        <v>85.8175</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>5</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Chandrasekharpur</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>20.3245</v>
+      </c>
+      <c r="E66" t="n">
+        <v>85.8185</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>6</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Niladri Vihar Square</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>20.316</v>
+      </c>
+      <c r="E67" t="n">
+        <v>85.819</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>7</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>VSS Nagar</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>20.301</v>
+      </c>
+      <c r="E68" t="n">
+        <v>85.845</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>8</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Rasulgarh Square</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>20.2885</v>
+      </c>
+      <c r="E69" t="n">
+        <v>85.86450000000001</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>9</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>VSS Nagar (Return)</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>20.3015</v>
+      </c>
+      <c r="E70" t="n">
+        <v>85.8455</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>10</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Niladri Vihar (Return)</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>20.3165</v>
+      </c>
+      <c r="E71" t="n">
+        <v>85.81950000000001</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>11</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Chandrasekharpur (Return)</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>20.325</v>
+      </c>
+      <c r="E72" t="n">
+        <v>85.819</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>12</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Damana Square (Return)</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>20.3345</v>
+      </c>
+      <c r="E73" t="n">
+        <v>85.818</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>13</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Patia Square (Return)</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>20.3448</v>
+      </c>
+      <c r="E74" t="n">
+        <v>85.8168</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>14</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>KIIT Square (Return)</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>20.351</v>
+      </c>
+      <c r="E75" t="n">
+        <v>85.819</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>15</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>KIIT Campus 25</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>20.3585</v>
+      </c>
+      <c r="E76" t="n">
+        <v>85.813</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
           <t>61</t>
         </is>
       </c>
-      <c r="B43" t="n">
-        <v>42</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>KIIT Campus 25</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>20.376</v>
-      </c>
-      <c r="E43" t="n">
-        <v>85.84</v>
+      <c r="B77" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>KIIT Transport Department</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>20.3524</v>
+      </c>
+      <c r="E77" t="n">
+        <v>85.8182</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>KIIT Campus 6</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>20.3508</v>
+      </c>
+      <c r="E78" t="n">
+        <v>85.8185</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>3</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>KIIT Campus 3</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>20.3501</v>
+      </c>
+      <c r="E79" t="n">
+        <v>85.81659999999999</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>4</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>KIMS</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>20.3495</v>
+      </c>
+      <c r="E80" t="n">
+        <v>85.81529999999999</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>5</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>KIIT International School</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>20.3425</v>
+      </c>
+      <c r="E81" t="n">
+        <v>85.81399999999999</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>6</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Silicon University</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>20.3513</v>
+      </c>
+      <c r="E82" t="n">
+        <v>85.80540000000001</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>7</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>DLF Cyber City</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>20.3552</v>
+      </c>
+      <c r="E83" t="n">
+        <v>85.8105</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>8</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Infocity Square</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>20.3568</v>
+      </c>
+      <c r="E84" t="n">
+        <v>85.8078</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>9</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Lord Jagannath Temple (S. Vihar)</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>20.3452</v>
+      </c>
+      <c r="E85" t="n">
+        <v>85.81950000000001</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>10</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Powergrid ER2 Odisha Projects</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>20.3345</v>
+      </c>
+      <c r="E86" t="n">
+        <v>85.8202</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>11</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Utkal Hospital</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>20.3242</v>
+      </c>
+      <c r="E87" t="n">
+        <v>85.8188</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>12</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Rail Vihar Road</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>20.3225</v>
+      </c>
+      <c r="E88" t="n">
+        <v>85.8192</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>13</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Kalinga Hospital Chowk</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>20.3204</v>
+      </c>
+      <c r="E89" t="n">
+        <v>85.8197</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>14</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Allen Career Institute</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>20.3122</v>
+      </c>
+      <c r="E90" t="n">
+        <v>85.8248</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>15</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Janta Maidan</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>20.3065</v>
+      </c>
+      <c r="E91" t="n">
+        <v>85.8265</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>16</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Pal Heights Mall</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>20.2982</v>
+      </c>
+      <c r="E92" t="n">
+        <v>85.8185</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>17</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Kalinga Stadium</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>20.2905</v>
+      </c>
+      <c r="E93" t="n">
+        <v>85.8201</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>18</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Raj Bhavan</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>20.2785</v>
+      </c>
+      <c r="E94" t="n">
+        <v>85.82250000000001</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>19</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Bana Durga Temple Road</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>20.2732</v>
+      </c>
+      <c r="E95" t="n">
+        <v>85.82550000000001</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>20</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Ekamra Niwas</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>20.2715</v>
+      </c>
+      <c r="E96" t="n">
+        <v>85.8288</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>21</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>AG Square</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>20.268</v>
+      </c>
+      <c r="E97" t="n">
+        <v>85.83199999999999</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>22</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Capital Hospital</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>20.2625</v>
+      </c>
+      <c r="E98" t="n">
+        <v>85.825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>